<commit_message>
Added ORM document for Project Plan in the directory.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>No</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Finish Date</t>
+  </si>
+  <si>
+    <t>RAM_MPP.doc</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,6 +450,15 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>10041802</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43200</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">

</xml_diff>

<commit_message>
Updated records for ORM documents and added new directories.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -33,10 +33,25 @@
     <t>Issue Date</t>
   </si>
   <si>
-    <t>Finish Date</t>
-  </si>
-  <si>
     <t>RAM_MPP.doc</t>
+  </si>
+  <si>
+    <t>RAM_TURS.doc</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Nay Lin Aung</t>
+  </si>
+  <si>
+    <t>Kaung Myat Bo</t>
+  </si>
+  <si>
+    <t>Balasubramanian</t>
+  </si>
+  <si>
+    <t>Closed Date</t>
   </si>
 </sst>
 </file>
@@ -85,10 +100,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -100,16 +116,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowCellStyle="Accent1">
-  <autoFilter ref="A1:E11">
-    <filterColumn colId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0" headerRowCellStyle="Accent1">
+  <autoFilter ref="A1:F23">
+    <filterColumn colId="3"/>
+    <filterColumn colId="5"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="No"/>
     <tableColumn id="2" name="ORM No"/>
     <tableColumn id="3" name="Review Document"/>
+    <tableColumn id="6" name="Author"/>
     <tableColumn id="4" name="Issue Date"/>
-    <tableColumn id="5" name="Finish Date"/>
+    <tableColumn id="5" name="Closed Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -400,22 +418,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -426,13 +444,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -442,11 +463,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
         <v>43177</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -454,51 +478,136 @@
         <v>10041802</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
         <v>43200</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="B4">
+        <v>15041803</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ORM records for reviews of MPP and WBS.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>No</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Risk Management Plan.doc</t>
+  </si>
+  <si>
+    <t>RAM_MWBS.xlsx</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,10 +532,34 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>17041805</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43207</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <v>17041806</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43207</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Updated ORM record for reviewing HLD.docx.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>No</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>RAM_MWBS.xlsx</t>
+  </si>
+  <si>
+    <t>HLD.docx</t>
+  </si>
+  <si>
+    <t>Treza Bawn Win</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,6 +571,18 @@
     <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
+      </c>
+      <c r="B8">
+        <v>22041807</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43212</v>
       </c>
     </row>
     <row r="9" spans="1:6">

</xml_diff>

<commit_message>
Updated ORM record for TUCMS.docx.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>No</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Treza Bawn Win</t>
+  </si>
+  <si>
+    <t>TUCMS.docs</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,6 +591,18 @@
     <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22081808</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>43212</v>
       </c>
     </row>
     <row r="10" spans="1:6">

</xml_diff>

<commit_message>
Added ORM_06051809_Prototype.doc for review of Prototype Study Report (PSR).
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>No</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>TUCMS.docs</t>
+  </si>
+  <si>
+    <t>06051809</t>
+  </si>
+  <si>
+    <t>Prototype_Draft.doc</t>
+  </si>
+  <si>
+    <t>GaoZuYi</t>
   </si>
 </sst>
 </file>
@@ -115,11 +124,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -436,7 +448,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -608,6 +620,18 @@
     <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43226</v>
       </c>
     </row>
     <row r="11" spans="1:6">

</xml_diff>

<commit_message>
Added records for ORM numbers issued for "TUCMS.docx" and "HLD.docx".
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>No</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>GaoZuYi</t>
+  </si>
+  <si>
+    <t>After 2nd Audit</t>
+  </si>
+  <si>
+    <t>Remark</t>
   </si>
 </sst>
 </file>
@@ -143,18 +149,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0" headerRowCellStyle="Accent1">
-  <autoFilter ref="A1:F23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G23" totalsRowShown="0" headerRowCellStyle="Accent1">
+  <autoFilter ref="A1:G23">
     <filterColumn colId="3"/>
     <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
   </autoFilter>
-  <tableColumns count="6">
+  <tableColumns count="7">
     <tableColumn id="1" name="No"/>
     <tableColumn id="2" name="ORM No"/>
     <tableColumn id="3" name="Review Document"/>
     <tableColumn id="6" name="Author"/>
     <tableColumn id="4" name="Issue Date"/>
     <tableColumn id="5" name="Closed Date"/>
+    <tableColumn id="7" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -445,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,10 +466,11 @@
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -480,8 +489,11 @@
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -497,8 +509,12 @@
       <c r="E2" s="1">
         <v>43177</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="1">
+        <v>43303</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -515,7 +531,7 @@
         <v>43200</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -532,7 +548,7 @@
         <v>43205</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -549,7 +565,7 @@
         <v>43205</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -566,7 +582,7 @@
         <v>43207</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -583,7 +599,7 @@
         <v>43207</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -600,7 +616,7 @@
         <v>43212</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -617,7 +633,7 @@
         <v>43212</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -634,32 +650,59 @@
         <v>43226</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="B11">
+        <v>31081810</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43343</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="B12">
+        <v>31081811</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -668,38 +711,39 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -708,6 +752,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated document records relating to reviews.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>No</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Remark</t>
+  </si>
+  <si>
+    <t>Risk Management Plan.docx</t>
+  </si>
+  <si>
+    <t>RAM_TURS.docx</t>
+  </si>
+  <si>
+    <t>RAM_MRP.xlsx</t>
+  </si>
+  <si>
+    <t>STP.docx</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -138,6 +150,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -456,7 +469,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,25 +704,69 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>17121812</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>43451</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>17121813</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1">
+        <v>43451</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>17121814</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>43451</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="3">
+        <v>17121815</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43451</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>

</xml_diff>

<commit_message>
Set "STP.docx" to baseline after review comment  incorporation.
Updated ORM records.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Review Records" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -472,7 +472,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -770,7 +770,9 @@
       <c r="E16" s="5">
         <v>43451</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="5">
+        <v>43470</v>
+      </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7">

</xml_diff>

<commit_message>
Issued ORM numbers for reviews and updated ORM review records.
</commit_message>
<xml_diff>
--- a/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
+++ b/MGMT/QUALITY/ORM/BASELINE/ORM_Records.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>No</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>RAM_MPP.docx</t>
+  </si>
+  <si>
+    <t>TUCMS.docx</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,10 +799,34 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>14011917</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>43479</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
+      </c>
+      <c r="B19">
+        <v>14011918</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>43479</v>
       </c>
     </row>
     <row r="20" spans="1:7">

</xml_diff>